<commit_message>
train in test data
</commit_message>
<xml_diff>
--- a/result/normVSstand.xlsx
+++ b/result/normVSstand.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\szeged\diplomamunka\pythonDiplomamunka\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7C1DF37-1DEA-4347-8CBB-2036C68AB019}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57D71B05-C81B-433F-9D4A-FAD2731CF119}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="allInOne" sheetId="5" r:id="rId1"/>
-    <sheet name="A1normVSstand" sheetId="1" r:id="rId2"/>
-    <sheet name="A5normVSstand" sheetId="3" r:id="rId3"/>
-    <sheet name="A10normVSstand" sheetId="4" r:id="rId4"/>
+    <sheet name="testVStrain" sheetId="7" r:id="rId1"/>
+    <sheet name="allInOne" sheetId="5" r:id="rId2"/>
+    <sheet name="A1normVSstand" sheetId="1" r:id="rId3"/>
+    <sheet name="A5normVSstand" sheetId="3" r:id="rId4"/>
+    <sheet name="A10normVSstand" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="resultsNorm" localSheetId="1">A1normVSstand!$A$1:$B$310</definedName>
-    <definedName name="resultsStand" localSheetId="3">A10normVSstand!$E$1:$F$310</definedName>
-    <definedName name="resultsStand" localSheetId="1">A1normVSstand!$E$1:$F$310</definedName>
-    <definedName name="resultsStand" localSheetId="2">A5normVSstand!$E$1:$F$310</definedName>
-    <definedName name="resultsStandA1" localSheetId="1">A1normVSstand!$O$1:$P$310</definedName>
+    <definedName name="resultsNorm" localSheetId="2">A1normVSstand!$A$1:$B$310</definedName>
+    <definedName name="resultsStand" localSheetId="4">A10normVSstand!$E$1:$F$310</definedName>
+    <definedName name="resultsStand" localSheetId="2">A1normVSstand!$E$1:$F$310</definedName>
+    <definedName name="resultsStand" localSheetId="3">A5normVSstand!$E$1:$F$310</definedName>
+    <definedName name="resultsStandA1" localSheetId="2">A1normVSstand!$O$1:$P$310</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="40">
   <si>
     <t xml:space="preserve">SVM complexity: </t>
   </si>
@@ -162,6 +163,45 @@
   </si>
   <si>
     <t>-a 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codebook settings are:  -normalizeInput, -a 5, -c random++, -norm 1, -size from 4096 to 32768 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">codebook settings are:  -normalizeInput, -a 10, -c random++, -norm 1, -size from 4096 to 32768 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">codebook settings are:  -standardizeInput, -a 5, -c random++, -norm 1, -size from 4096 to 32768 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">codebook settings are:  -standardizeInput, -a 10, -c random++, -norm 1, -size from 4096 to 32768 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test database UAR: </t>
+  </si>
+  <si>
+    <t>train UAR</t>
+  </si>
+  <si>
+    <t>test UAR</t>
+  </si>
+  <si>
+    <t>testUAR</t>
+  </si>
+  <si>
+    <t>trainUAR</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>normalize</t>
+  </si>
+  <si>
+    <t>standardize</t>
+  </si>
+  <si>
+    <t>a10</t>
   </si>
 </sst>
 </file>
@@ -860,7 +900,49 @@
     <cellStyle name="Semleges" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Számítás" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -917,23 +999,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsNorm" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="4" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStandA1" connectionId="7" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStandA1" connectionId="7" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsNorm" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="5" xr16:uid="{00000000-0016-0000-0100-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="5" xr16:uid="{00000000-0016-0000-0200-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="6" xr16:uid="{00000000-0016-0000-0200-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="resultsStand" connectionId="6" xr16:uid="{00000000-0016-0000-0300-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1232,592 +1314,3665 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5444CE8-CD35-4EB5-A428-ED92A60A2BC5}">
-  <dimension ref="B2:R14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2648F6-3F2D-417E-A118-62E1A9D477E3}">
+  <dimension ref="A1:S155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:R17"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="18" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D2" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="R3" s="23"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="24">
-        <v>0.53787654224008097</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="36">
+    <row r="1" spans="1:19" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.86761331038439404</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.85676993689041803</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.87485656913367704</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0.862808376362593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.70806376535997595</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.68119213529300005</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.708613434591711</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>0.70200946870852998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.60529189087915802</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.58031309892378002</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.602135854341736</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>0.58026348039215603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.86887550200803199</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.87000860585197903</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.86404188181296604</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>0.86640849110728602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.71966152660292504</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.69989842643758904</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.68947961731422003</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>0.69792591098899204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.61885422111428301</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="36">
+      <c r="F12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.67987259816207102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.59397307933008403</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0.58987394957983097</v>
+      </c>
+      <c r="S12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="D13">
+        <f>MAX(B6,B11,B16,B21,B26,B31,B36)</f>
+        <v>0.71966152660292504</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13">
+        <f>MAX(G6,G11,G16,G21,G26,G31,G36)</f>
+        <v>0.73164182847191905</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="N13">
+        <f>MAX(L6,L11,L16,L21,L26,L31,L36)</f>
+        <v>0.72947401827271996</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="S13">
+        <f>MAX(Q6,Q11,Q16,Q21,Q26,Q31,Q36)</f>
+        <v>0.71597035160206501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="S14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.86521801491681005</v>
+      </c>
+      <c r="D15">
+        <f>MAX(B7,B12,B17,B22,B27,B32,B37)</f>
+        <v>0.688612637362637</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.86639414802065395</v>
+      </c>
+      <c r="I15">
+        <f>MAX(G7,G12,G17,G22,G27,G32,G37)</f>
+        <v>0.67987259816207102</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.86880378657487101</v>
+      </c>
+      <c r="N15">
+        <f>MAX(L7,L12,L17,L22,L27,L32,L37)</f>
+        <v>0.646308558035531</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0.85806081468731998</v>
+      </c>
+      <c r="S15">
+        <f>MAX(Q7,Q12,Q17,Q22,Q27,Q32,Q37)</f>
+        <v>0.62863782459370598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.70951089626797603</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.71586895019836705</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.72947401827271996</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0.70880095692282796</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.64986470977279798</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0.60546792328042298</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0.646308558035531</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0.57802414021163995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.86277969018932799</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0.86884681583476697</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0.86041308089500801</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0.86880378657487101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.70833310846872899</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.70205430258764201</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0.69657555618487899</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.71597035160206501</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.61832603874883196</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.60880733087002403</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0.63313148656898599</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>0.606307360510146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7">
         <v>0.1</v>
       </c>
-      <c r="F4" s="24">
-        <v>0.50194806170638195</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.50620604949061798</v>
-      </c>
-      <c r="I4" s="36">
+      <c r="F24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7">
         <v>0.1</v>
       </c>
-      <c r="J4" s="36">
+      <c r="K24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.853141135972461</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.86878944348823794</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="7">
+        <v>0.86164658634538105</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.86288009179575398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.67575987017468298</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.70540957912501501</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0.71005466889978996</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0.69051269019403505</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.63252287404860896</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.67194723509061705</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0.61035290077569404</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0.59876958020050097</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.85915088927137095</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.865232358003442</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0.86045611015490497</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>0.86288009179575398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.71779302562454905</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0.73164182847191905</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0.67199065075147102</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0.69644853514551797</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.59040952103452105</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0.67239845938375298</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0.58666888924628802</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0.60612190709617098</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="7">
+        <v>10</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7">
+        <v>10</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
+        <v>10</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.85919391853126703</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.86285140562248996</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0.86399885255306896</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0.85806081468731998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.68272045951693505</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0.69988168451302202</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.72406964802426299</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0.70076213510820495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.688612637362637</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="7">
+        <v>0.66770731278954898</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L37" s="7">
+        <v>0.63470654861134701</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0.62863782459370598</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0.86764199655765895</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.86639414802065395</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="5">
+        <v>0.85444635685599502</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>0.86640849110728602</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.71532559399978302</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0.70003622083316197</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0.69676105905351005</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>0.72296078753881898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.64009199445635201</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.63067564745196303</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L42" s="5">
+        <v>0.57484079377364905</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>0.66422277176727595</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.86527538726333897</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.86520367183017799</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0.86283706253585701</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>0.86288009179575398</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.68932311180285599</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0.69714990627270301</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L46" s="5">
+        <v>0.69242603657520396</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>0.680907357106452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.66886021658080397</v>
+      </c>
+      <c r="D47" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="36">
+      <c r="F47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.64251722950252299</v>
+      </c>
+      <c r="I47" t="s">
+        <v>32</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L47" s="5">
+        <v>0.61375911261940597</v>
+      </c>
+      <c r="N47" t="s">
+        <v>32</v>
+      </c>
+      <c r="P47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>0.66562935022493797</v>
+      </c>
+      <c r="S47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="D48">
+        <f>MAX(B41,B46,B51,B56,B61,B66,B71)</f>
+        <v>0.73527238200424405</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="I48">
+        <f>MAX(G41,G46,G51,G56,G61,G66,G71)</f>
+        <v>0.72752111674156195</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="N48">
+        <f>MAX(L41,L46,L51,L56,L61,L66,L71)</f>
+        <v>0.73080745544986603</v>
+      </c>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="S48">
+        <f>MAX(Q41,Q46,Q51,Q56,Q61,Q66,Q71)</f>
+        <v>0.72296078753881898</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="5">
         <v>1E-3</v>
       </c>
-      <c r="L4" s="24">
-        <v>0.51205746388238105</v>
-      </c>
-      <c r="N4" s="24">
-        <v>0.49364470749071798</v>
-      </c>
-      <c r="O4" s="36">
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="N49" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0.86765633964429101</v>
+      </c>
+      <c r="D50">
+        <f>MAX(B42,B47,B52,B57,B62,B67,B72)</f>
+        <v>0.73435574186735098</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0.86768502581755502</v>
+      </c>
+      <c r="I50">
+        <f>MAX(G42,G47,G52,G57,G62,G67,G72)</f>
+        <v>0.66429682857991601</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L50" s="5">
+        <v>0.86285140562248996</v>
+      </c>
+      <c r="N50">
+        <f>MAX(L42,L47,L52,L57,L62,L67,L72)</f>
+        <v>0.68871723323832401</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>0.86401319563970103</v>
+      </c>
+      <c r="S50">
+        <f>MAX(Q42,Q47,Q52,Q57,Q62,Q67,Q72)</f>
+        <v>0.66562935022493797</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0.69608446129481905</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0.71835239215820701</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L51" s="5">
+        <v>0.71758878671395299</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>0.68955415840019496</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0.61574746342838405</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.60404239658690095</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L52" s="5">
+        <v>0.62849946622005404</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>0.61937523626184599</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0.86649454962707895</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" s="5">
+        <v>0.86758462421113003</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" s="5">
+        <v>0.86279403327596005</v>
+      </c>
+      <c r="P55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>0.85434595524956902</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.73527238200424405</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0.71127272040586498</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L56" s="5">
+        <v>0.72393720705445397</v>
+      </c>
+      <c r="P56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>0.69078037957677596</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0.70803668689698096</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="5">
+        <v>0.64449334026539895</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L57" s="5">
+        <v>0.64041155603655597</v>
+      </c>
+      <c r="P57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>0.63433463648924104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L59" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="P59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0.87122776821572001</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="5">
+        <v>0.87122776821572001</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L60" s="5">
+        <v>0.85806081468731998</v>
+      </c>
+      <c r="P60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>0.86270797475616701</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.71056660419456896</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="5">
+        <v>0.72752111674156195</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61" s="5">
+        <v>0.693006634965319</v>
+      </c>
+      <c r="P61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q61" s="5">
+        <v>0.70159645504804502</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0.625097621032218</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" s="5">
+        <v>0.64298406862744995</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L62" s="5">
+        <v>0.62792758969616502</v>
+      </c>
+      <c r="P62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>0.61003283889313298</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="5">
+        <v>1</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" s="5">
+        <v>1</v>
+      </c>
+      <c r="P64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="5">
+        <v>0.86402753872633398</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G65" s="5">
+        <v>0.86158921399885202</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L65" s="5">
+        <v>0.85557946069994195</v>
+      </c>
+      <c r="P65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>0.86762765347102599</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0.72174264379549602</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G66" s="5">
+        <v>0.68734775480662103</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L66" s="5">
+        <v>0.68708275532602003</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q66" s="5">
+        <v>0.71924217431321302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="5">
+        <v>0.69087171052631502</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G67" s="5">
+        <v>0.62939072623283099</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L67" s="5">
+        <v>0.61805249950857499</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q67" s="5">
+        <v>0.63401937236882999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="5">
+        <v>10</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" s="5">
+        <v>10</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L69" s="5">
+        <v>10</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="5">
+        <v>0.86160355708548397</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" s="5">
+        <v>0.86649454962707895</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L70" s="5">
+        <v>0.86270797475616701</v>
+      </c>
+      <c r="P70" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="5">
+        <v>0.86038439472174399</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="5">
+        <v>0.69247787560262297</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="5">
+        <v>0.71958311763375704</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L71" s="5">
+        <v>0.73080745544986603</v>
+      </c>
+      <c r="P71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q71" s="5">
+        <v>0.70997390639445701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0.73435574186735098</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="5">
+        <v>0.66429682857991601</v>
+      </c>
+      <c r="K72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L72" s="5">
+        <v>0.68871723323832401</v>
+      </c>
+      <c r="P72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q72" s="5">
+        <v>0.61618228381095996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="10">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="P4" s="36">
+      <c r="F74" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="10">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K74" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L74" s="10">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P74" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="10">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="9">
+        <v>0.86163224325874899</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G75" s="9">
+        <v>0.86160355708548397</v>
+      </c>
+      <c r="K75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L75" s="9">
+        <v>0.86402753872633398</v>
+      </c>
+      <c r="P75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="9">
+        <v>0.86407056798623005</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="9">
+        <v>0.70849117423522701</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G76" s="9">
+        <v>0.69518665938188895</v>
+      </c>
+      <c r="K76" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0.70836125214961598</v>
+      </c>
+      <c r="P76" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>0.69971020633869996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="9">
+        <v>0.63996603327872603</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" s="9">
+        <v>0.62260941876750697</v>
+      </c>
+      <c r="K77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L77" s="9">
+        <v>0.61758145363408501</v>
+      </c>
+      <c r="P77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q77" s="9">
+        <v>0.61314891506841895</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G79" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="K79" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L79" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="P79" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="9">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="9">
+        <v>0.85679862306368304</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G80" s="9">
+        <v>0.86761331038439404</v>
+      </c>
+      <c r="K80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L80" s="9">
+        <v>0.85925129087779595</v>
+      </c>
+      <c r="P80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="9">
+        <v>0.86520367183017699</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="9">
+        <v>0.70830432103999497</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G81" s="9">
+        <v>0.70864839919724998</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L81" s="9">
+        <v>0.70442229870724904</v>
+      </c>
+      <c r="P81" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q81" s="9">
+        <v>0.72635639980353295</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="9">
+        <v>0.67195196798815204</v>
+      </c>
+      <c r="D82" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="24">
-        <v>0.50497990709548901</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="25">
-        <v>0.51888184922566505</v>
-      </c>
-      <c r="C5" s="36">
+      <c r="F82" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="9">
+        <v>0.68946794068504602</v>
+      </c>
+      <c r="I82" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L82" s="9">
+        <v>0.63273272353864396</v>
+      </c>
+      <c r="N82" t="s">
+        <v>32</v>
+      </c>
+      <c r="P82" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q82" s="9">
+        <v>0.64523511833883296</v>
+      </c>
+      <c r="S82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="D83">
+        <f>MAX(B76,B81,B86,B91,B96,B101,B106)</f>
+        <v>0.73497941084274698</v>
+      </c>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="I83">
+        <f>MAX(G76,G81,G86,G91,G96,G101,G106)</f>
+        <v>0.719437462952218</v>
+      </c>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="N83">
+        <f>MAX(L76,L81,L86,L91,L96,L101,L106)</f>
+        <v>0.71938898103992399</v>
+      </c>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="9"/>
+      <c r="S83">
+        <f>MAX(Q76,Q81,Q86,Q91,Q96,Q101,Q106)</f>
+        <v>0.72918125537633904</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>33</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G84" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I84" t="s">
+        <v>33</v>
+      </c>
+      <c r="K84" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L84" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="N84" t="s">
+        <v>33</v>
+      </c>
+      <c r="P84" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="S84" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="9">
+        <v>0.86037005163511104</v>
+      </c>
+      <c r="D85">
+        <f>MAX(B77,B82,B87,B92,B97,B102,B107)</f>
+        <v>0.67389256576756495</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G85" s="9">
+        <v>0.86636546184738905</v>
+      </c>
+      <c r="I85">
+        <f>MAX(G77,G82,G87,G92,G97,G102,G107)</f>
+        <v>0.68946794068504602</v>
+      </c>
+      <c r="K85" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L85" s="9">
+        <v>0.859136546184739</v>
+      </c>
+      <c r="N85">
+        <f>MAX(L77,L82,L87,L92,L97,L102,L107)</f>
+        <v>0.63273272353864396</v>
+      </c>
+      <c r="P85" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>0.86283706253585701</v>
+      </c>
+      <c r="S85">
+        <f>MAX(Q77,Q82,Q87,Q92,Q97,Q102,Q107)</f>
+        <v>0.67388759889920802</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="9">
+        <v>0.69576154215271402</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G86" s="9">
+        <v>0.713284876666474</v>
+      </c>
+      <c r="K86" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L86" s="9">
+        <v>0.69675795433990195</v>
+      </c>
+      <c r="P86" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>0.72918125537633904</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="9">
+        <v>0.67389256576756495</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G87" s="9">
+        <v>0.68093980215690697</v>
+      </c>
+      <c r="K87" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L87" s="9">
+        <v>0.60874676385705795</v>
+      </c>
+      <c r="P87" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q87" s="9">
+        <v>0.61671580215020605</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="P88" s="9"/>
+      <c r="Q88" s="9"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="9">
         <v>0.01</v>
       </c>
-      <c r="D5" s="36">
-        <v>64</v>
-      </c>
-      <c r="E5" s="36">
+      <c r="F89" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G89" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K89" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L89" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="P89" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="9">
+        <v>0.85801778542742402</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" s="9">
+        <v>0.86520367183017799</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L90" s="9">
+        <v>0.86759896729776198</v>
+      </c>
+      <c r="P90" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="9">
+        <v>0.86160355708548397</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="9">
+        <v>0.716028928369985</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G91" s="9">
+        <v>0.719437462952218</v>
+      </c>
+      <c r="K91" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L91" s="9">
+        <v>0.71938898103992399</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q91" s="9">
+        <v>0.71275307667355503</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B92" s="9">
+        <v>0.64894494394494295</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G92" s="9">
+        <v>0.63124273398170405</v>
+      </c>
+      <c r="K92" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L92" s="9">
+        <v>0.60863044624364204</v>
+      </c>
+      <c r="P92" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q92" s="9">
+        <v>0.67388759889920802</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="9"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="9">
         <v>0.1</v>
       </c>
-      <c r="F5" s="25">
-        <v>0.51944949899059201</v>
-      </c>
-      <c r="H5" s="25">
-        <v>0.53433369351518101</v>
-      </c>
-      <c r="I5" s="36">
+      <c r="F94" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G94" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L94" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="P94" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="9">
+        <v>0.85679862306368304</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G95" s="9">
+        <v>0.86398450946643701</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L95" s="9">
+        <v>0.86401319563970103</v>
+      </c>
+      <c r="P95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="9">
+        <v>0.85557946069994195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="9">
+        <v>0.68968052160563698</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G96" s="9">
+        <v>0.71008808117653599</v>
+      </c>
+      <c r="K96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L96" s="9">
+        <v>0.71262092338795602</v>
+      </c>
+      <c r="P96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q96" s="9">
+        <v>0.69471525981959403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97" s="9">
+        <v>0.65093598803157604</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" s="9">
+        <v>0.67499026010539098</v>
+      </c>
+      <c r="K97" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L97" s="9">
+        <v>0.53483173076922996</v>
+      </c>
+      <c r="P97" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q97" s="9">
+        <v>0.61497343299974805</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+      <c r="P98" s="9"/>
+      <c r="Q98" s="9"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="9">
+        <v>1</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G99" s="9">
+        <v>1</v>
+      </c>
+      <c r="K99" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L99" s="9">
+        <v>1</v>
+      </c>
+      <c r="P99" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="9">
+        <v>0.86163224325874899</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G100" s="9">
+        <v>0.86402753872633398</v>
+      </c>
+      <c r="K100" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L100" s="9">
+        <v>0.85912220309810605</v>
+      </c>
+      <c r="P100" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="9">
+        <v>0.85794606999426204</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="9">
+        <v>0.71925072323200201</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G101" s="9">
+        <v>0.69348515404020405</v>
+      </c>
+      <c r="K101" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L101" s="9">
+        <v>0.70006961405591905</v>
+      </c>
+      <c r="P101" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q101" s="9">
+        <v>0.71171006555873595</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" s="9">
+        <v>0.63046303369832701</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" s="9">
+        <v>0.63475629433059699</v>
+      </c>
+      <c r="K102" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L102" s="9">
+        <v>0.60749598902559399</v>
+      </c>
+      <c r="P102" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q102" s="9">
+        <v>0.66684934400394902</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="9"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="9">
+        <v>10</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G104" s="9">
+        <v>10</v>
+      </c>
+      <c r="K104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L104" s="9">
+        <v>10</v>
+      </c>
+      <c r="P104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="9">
+        <v>0.86765633964429101</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G105" s="9">
+        <v>0.86157487091221996</v>
+      </c>
+      <c r="K105" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L105" s="9">
+        <v>0.86156052782558801</v>
+      </c>
+      <c r="P105" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="9">
+        <v>0.86276534710269603</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="9">
+        <v>0.73497941084274698</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G106" s="9">
+        <v>0.70103647765867405</v>
+      </c>
+      <c r="K106" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L106" s="9">
+        <v>0.700388984684156</v>
+      </c>
+      <c r="P106" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q106" s="9">
+        <v>0.709891877042226</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B107" s="9">
+        <v>0.66722484827264195</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G107" s="9">
+        <v>0.63302002531781898</v>
+      </c>
+      <c r="K107" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L107" s="9">
+        <v>0.62564149343948094</v>
+      </c>
+      <c r="P107" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q107" s="9">
+        <v>0.61068452380952298</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F109" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G109" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K109" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L109" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P109" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="11">
+        <v>0.86642283419391797</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" s="11">
+        <v>0.86037005163511204</v>
+      </c>
+      <c r="K110" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L110" s="11">
+        <v>0.86520367183017799</v>
+      </c>
+      <c r="P110" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q110" s="11">
+        <v>0.86887550200803199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="11">
+        <v>0.72767793730701202</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G111" s="11">
+        <v>0.69812844189019996</v>
+      </c>
+      <c r="K111" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L111" s="11">
+        <v>0.72985377134388796</v>
+      </c>
+      <c r="P111" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q111" s="11">
+        <v>0.73821199293098805</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="11">
+        <v>0.74551247911445195</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G112" s="11">
+        <v>0.72035313188273697</v>
+      </c>
+      <c r="K112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L112" s="11">
+        <v>0.67569736227824395</v>
+      </c>
+      <c r="P112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q112" s="11">
+        <v>0.62243055555555504</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="11"/>
+      <c r="K113" s="11"/>
+      <c r="L113" s="11"/>
+      <c r="P113" s="11"/>
+      <c r="Q113" s="11"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G114" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="K114" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L114" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="P114" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q114" s="11">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B115" s="11">
+        <v>0.87125645438898403</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G115" s="11">
+        <v>0.86768502581755602</v>
+      </c>
+      <c r="K115" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L115" s="11">
+        <v>0.85800344234079096</v>
+      </c>
+      <c r="P115" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q115" s="11">
+        <v>0.86277969018932799</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="11">
+        <v>0.728751365955424</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G116" s="11">
+        <v>0.71109424824466105</v>
+      </c>
+      <c r="K116" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L116" s="11">
+        <v>0.70492557545527901</v>
+      </c>
+      <c r="P116" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q116" s="11">
+        <v>0.70715554944705195</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B117" s="11">
+        <v>0.71138049450549401</v>
+      </c>
+      <c r="D117" t="s">
+        <v>32</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G117" s="11">
+        <v>0.694400987192202</v>
+      </c>
+      <c r="I117" t="s">
+        <v>32</v>
+      </c>
+      <c r="K117" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L117" s="11">
+        <v>0.60456194755536796</v>
+      </c>
+      <c r="N117" t="s">
+        <v>32</v>
+      </c>
+      <c r="P117" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q117" s="11">
+        <v>0.64449826725561998</v>
+      </c>
+      <c r="S117" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
+      <c r="D118">
+        <f>MAX(B111,B116,B121,B126,B131,B136,B141)</f>
+        <v>0.728751365955424</v>
+      </c>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+      <c r="I118">
+        <f>MAX(G111,G116,G121,G126,G131,G136,G141)</f>
+        <v>0.74653592343395603</v>
+      </c>
+      <c r="K118" s="11"/>
+      <c r="L118" s="11"/>
+      <c r="N118">
+        <f>MAX(L111,L116,L121,L126,L131,L136,L141)</f>
+        <v>0.73686805872075301</v>
+      </c>
+      <c r="P118" s="11"/>
+      <c r="Q118" s="11"/>
+      <c r="S118">
+        <f>MAX(Q111,Q116,Q121,Q126,Q131,Q136,Q141)</f>
+        <v>0.73821199293098805</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="11">
         <v>1E-3</v>
       </c>
-      <c r="J5" s="36">
-        <v>64</v>
-      </c>
-      <c r="K5" s="36">
+      <c r="D119" t="s">
+        <v>33</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G119" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="I119" t="s">
+        <v>33</v>
+      </c>
+      <c r="K119" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L119" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="N119" t="s">
+        <v>33</v>
+      </c>
+      <c r="P119" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q119" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="S119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="11">
+        <v>0.87481353987377997</v>
+      </c>
+      <c r="D120">
+        <f>MAX(B112,B117,B122,B127,B132,B137,B142)</f>
+        <v>0.74551247911445195</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G120" s="11">
+        <v>0.85674125071715401</v>
+      </c>
+      <c r="I120">
+        <f>MAX(G112,G117,G122,G127,G132,G137,G142)</f>
+        <v>0.72035313188273697</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L120" s="11">
+        <v>0.86411359724612702</v>
+      </c>
+      <c r="N120">
+        <f>MAX(L112,L117,L122,L127,L132,L137,L142)</f>
+        <v>0.70879909360075699</v>
+      </c>
+      <c r="P120" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q120" s="11">
+        <v>0.86886115892139903</v>
+      </c>
+      <c r="S120">
+        <f>MAX(Q112,Q117,Q122,Q127,Q132,Q137,Q142)</f>
+        <v>0.69586431295312801</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="11">
+        <v>0.71162794233418203</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G121" s="11">
+        <v>0.67489143151409303</v>
+      </c>
+      <c r="K121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L121" s="11">
+        <v>0.72414538076677504</v>
+      </c>
+      <c r="P121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q121" s="11">
+        <v>0.71881319831997903</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B122" s="11">
+        <v>0.67741831246668704</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G122" s="11">
+        <v>0.71306568499583201</v>
+      </c>
+      <c r="K122" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L122" s="11">
+        <v>0.62161457007045195</v>
+      </c>
+      <c r="P122" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q122" s="11">
+        <v>0.65469957061771999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="F123" s="11"/>
+      <c r="G123" s="11"/>
+      <c r="K123" s="11"/>
+      <c r="L123" s="11"/>
+      <c r="P123" s="11"/>
+      <c r="Q123" s="11"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="11">
         <v>0.01</v>
       </c>
-      <c r="L5" s="25">
-        <v>0.52818466098865702</v>
-      </c>
-      <c r="N5" s="25">
-        <v>0.560864808066181</v>
-      </c>
-      <c r="O5" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="P5" s="36">
-        <v>64</v>
-      </c>
-      <c r="Q5" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="R5" s="25">
-        <v>0.53285754431889698</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="26">
-        <v>0.610294673678907</v>
-      </c>
-      <c r="C6" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="D6" s="36">
-        <v>128</v>
-      </c>
-      <c r="E6" s="36">
+      <c r="F124" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G124" s="11">
         <v>0.01</v>
       </c>
-      <c r="F6" s="26">
-        <v>0.53332500398919103</v>
-      </c>
-      <c r="H6" s="26">
-        <v>0.57033623380503795</v>
-      </c>
-      <c r="I6" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="J6" s="36">
-        <v>128</v>
-      </c>
-      <c r="K6" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="L6" s="26">
-        <v>0.53488996995256799</v>
-      </c>
-      <c r="N6" s="26">
-        <v>0.583551808633887</v>
-      </c>
-      <c r="O6" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="P6" s="36">
-        <v>128</v>
-      </c>
-      <c r="Q6" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="R6" s="26">
-        <v>0.54176305677466097</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="27">
-        <v>0.61310887218439902</v>
-      </c>
-      <c r="C7" s="36">
+      <c r="K124" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L124" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="P124" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="11">
+        <v>0.86157487091221996</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G125" s="11">
+        <v>0.86034136546184703</v>
+      </c>
+      <c r="K125" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L125" s="11">
+        <v>0.85196500286861698</v>
+      </c>
+      <c r="P125" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q125" s="11">
+        <v>0.85804647160068803</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="11">
+        <v>0.70262848487424501</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G126" s="11">
+        <v>0.67440102259262003</v>
+      </c>
+      <c r="K126" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L126" s="11">
+        <v>0.68143496549006</v>
+      </c>
+      <c r="P126" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q126" s="11">
+        <v>0.69839485948775004</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B127" s="11">
+        <v>0.67744407456578504</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G127" s="11">
+        <v>0.660736580670791</v>
+      </c>
+      <c r="K127" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L127" s="11">
+        <v>0.65861277990728395</v>
+      </c>
+      <c r="P127" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q127" s="11">
+        <v>0.67030753968253898</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="F128" s="11"/>
+      <c r="G128" s="11"/>
+      <c r="K128" s="11"/>
+      <c r="L128" s="11"/>
+      <c r="P128" s="11"/>
+      <c r="Q128" s="11"/>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A129" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F129" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G129" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="K129" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L129" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="P129" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A130" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B130" s="11">
+        <v>0.86521801491681005</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G130" s="11">
+        <v>0.86764199655765895</v>
+      </c>
+      <c r="K130" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L130" s="11">
+        <v>0.84846528973034996</v>
+      </c>
+      <c r="P130" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="11">
+        <v>0.85797475616752705</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A131" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="11">
+        <v>0.71967692224916502</v>
+      </c>
+      <c r="F131" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G131" s="11">
+        <v>0.72380950484394302</v>
+      </c>
+      <c r="K131" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L131" s="11">
+        <v>0.702396884857032</v>
+      </c>
+      <c r="P131" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q131" s="11">
+        <v>0.71002214031998401</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A132" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B132" s="11">
+        <v>0.71442379515908905</v>
+      </c>
+      <c r="F132" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G132" s="11">
+        <v>0.62675168581418506</v>
+      </c>
+      <c r="K132" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L132" s="11">
+        <v>0.65793045447844201</v>
+      </c>
+      <c r="P132" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q132" s="11">
+        <v>0.613982524828113</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A133" s="11"/>
+      <c r="B133" s="11"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+      <c r="K133" s="11"/>
+      <c r="L133" s="11"/>
+      <c r="P133" s="11"/>
+      <c r="Q133" s="11"/>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A134" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="11">
+        <v>1</v>
+      </c>
+      <c r="F134" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G134" s="11">
+        <v>1</v>
+      </c>
+      <c r="K134" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L134" s="11">
+        <v>1</v>
+      </c>
+      <c r="P134" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A135" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B135" s="11">
+        <v>0.86401319563970103</v>
+      </c>
+      <c r="F135" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G135" s="11">
+        <v>0.87479919678714801</v>
+      </c>
+      <c r="K135" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L135" s="11">
+        <v>0.85193631669535197</v>
+      </c>
+      <c r="P135" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q135" s="11">
+        <v>0.86038439472174399</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A136" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B136" s="11">
+        <v>0.69858618763890801</v>
+      </c>
+      <c r="F136" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="11">
+        <v>0.74653592343395603</v>
+      </c>
+      <c r="K136" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L136" s="11">
+        <v>0.70368537031043099</v>
+      </c>
+      <c r="P136" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q136" s="11">
+        <v>0.70707681961227797</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B137" s="11">
+        <v>0.70003698482316901</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G137" s="11">
+        <v>0.71066512263106696</v>
+      </c>
+      <c r="K137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L137" s="11">
+        <v>0.66545282536091299</v>
+      </c>
+      <c r="P137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q137" s="11">
+        <v>0.58620266687217104</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
+      <c r="F138" s="11"/>
+      <c r="G138" s="11"/>
+      <c r="K138" s="11"/>
+      <c r="L138" s="11"/>
+      <c r="P138" s="11"/>
+      <c r="Q138" s="11"/>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A139" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="11">
         <v>10</v>
       </c>
-      <c r="D7" s="36">
-        <v>256</v>
-      </c>
-      <c r="E7" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="F7" s="27">
-        <v>0.59040029968531405</v>
-      </c>
-      <c r="H7" s="27">
-        <v>0.64945044609913505</v>
-      </c>
-      <c r="I7" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="36">
-        <v>256</v>
-      </c>
-      <c r="K7" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="L7" s="27">
-        <v>0.62286818119687304</v>
-      </c>
-      <c r="N7" s="27">
-        <v>0.63333478582543201</v>
-      </c>
-      <c r="O7" s="36">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="P7" s="36">
-        <v>256</v>
-      </c>
-      <c r="Q7" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="R7" s="27">
-        <v>0.58681249297936</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="41">
-        <v>0.62254876362313305</v>
-      </c>
-      <c r="C8" s="42">
+      <c r="F139" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G139" s="11">
         <v>10</v>
       </c>
-      <c r="D8" s="42">
-        <v>512</v>
-      </c>
-      <c r="E8" s="42">
-        <v>1E-4</v>
-      </c>
-      <c r="F8" s="41">
-        <v>0.61549172196306701</v>
-      </c>
-      <c r="H8" s="41">
-        <v>0.65684570485080496</v>
-      </c>
-      <c r="I8" s="42">
-        <v>1E-4</v>
-      </c>
-      <c r="J8" s="42">
-        <v>512</v>
-      </c>
-      <c r="K8" s="42">
-        <v>0.01</v>
-      </c>
-      <c r="L8" s="41">
-        <v>0.62443421273978905</v>
-      </c>
-      <c r="N8" s="41">
-        <v>0.64372310217745499</v>
-      </c>
-      <c r="O8" s="42">
-        <v>1E-4</v>
-      </c>
-      <c r="P8" s="42">
-        <v>512</v>
-      </c>
-      <c r="Q8" s="42">
+      <c r="K139" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L139" s="11">
         <v>10</v>
       </c>
-      <c r="R8" s="41">
-        <v>0.63689972433987196</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="29">
-        <v>0.645481346780578</v>
-      </c>
-      <c r="C9" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="36">
-        <v>1024</v>
-      </c>
-      <c r="E9" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="F9" s="29">
-        <v>0.67052074001526396</v>
-      </c>
-      <c r="H9" s="29">
-        <v>0.69483838922529395</v>
-      </c>
-      <c r="I9" s="36">
-        <v>1</v>
-      </c>
-      <c r="J9" s="36">
-        <v>1024</v>
-      </c>
-      <c r="K9" s="36">
-        <v>1</v>
-      </c>
-      <c r="L9" s="29">
-        <v>0.66266973483061897</v>
-      </c>
-      <c r="N9" s="29">
-        <v>0.709722222322271</v>
-      </c>
-      <c r="O9" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="P9" s="36">
-        <v>1024</v>
-      </c>
-      <c r="Q9" s="36">
-        <v>1E-4</v>
-      </c>
-      <c r="R9" s="29">
-        <v>0.66967553814540504</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="30">
-        <v>0.694987655095329</v>
-      </c>
-      <c r="C10" s="36">
-        <v>1</v>
-      </c>
-      <c r="D10" s="36">
-        <v>2048</v>
-      </c>
-      <c r="E10" s="36">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0.66531969031195404</v>
-      </c>
-      <c r="H10" s="30">
-        <v>0.71015245992759202</v>
-      </c>
-      <c r="I10" s="36">
-        <v>1E-3</v>
-      </c>
-      <c r="J10" s="36">
-        <v>2048</v>
-      </c>
-      <c r="K10" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="30">
-        <v>0.703051004096238</v>
-      </c>
-      <c r="N10" s="30">
-        <v>0.69871846339354704</v>
-      </c>
-      <c r="O10" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="36">
-        <v>2048</v>
-      </c>
-      <c r="Q10" s="36">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R10" s="30">
-        <v>0.72089388717042102</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44">
-        <v>0.68707097943421502</v>
-      </c>
-      <c r="C11" s="45">
-        <v>0.01</v>
-      </c>
-      <c r="D11" s="45">
+      <c r="P139" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A140" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="11">
+        <v>0.86401319563970103</v>
+      </c>
+      <c r="F140" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G140" s="11">
+        <v>0.86764199655765895</v>
+      </c>
+      <c r="K140" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L140" s="11">
+        <v>0.86531841652323505</v>
+      </c>
+      <c r="P140" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="11">
+        <v>0.85318416523235696</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="11">
+        <v>0.72229052432308205</v>
+      </c>
+      <c r="F141" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G141" s="11">
+        <v>0.71232643202132195</v>
+      </c>
+      <c r="K141" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L141" s="11">
+        <v>0.73686805872075301</v>
+      </c>
+      <c r="P141" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q141" s="11">
+        <v>0.68791626757479996</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A142" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B142" s="11">
+        <v>0.68122405920103202</v>
+      </c>
+      <c r="F142" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G142" s="11">
+        <v>0.67352593753425705</v>
+      </c>
+      <c r="K142" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L142" s="11">
+        <v>0.70879909360075699</v>
+      </c>
+      <c r="P142" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q142" s="11">
+        <v>0.69586431295312801</v>
+      </c>
+    </row>
+    <row r="147" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>34</v>
+      </c>
+      <c r="D147" t="s">
+        <v>35</v>
+      </c>
+      <c r="H147" t="s">
+        <v>34</v>
+      </c>
+      <c r="I147" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="148" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B148">
         <v>4096</v>
       </c>
-      <c r="E11" s="45">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="F11" s="44">
-        <v>0.67799559054648895</v>
-      </c>
-      <c r="H11" s="44">
-        <v>0.71692056356342004</v>
-      </c>
-      <c r="I11" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="45">
+      <c r="C148">
+        <f>D$15</f>
+        <v>0.688612637362637</v>
+      </c>
+      <c r="D148">
+        <f>D$13</f>
+        <v>0.71966152660292504</v>
+      </c>
+      <c r="G148">
         <v>4096</v>
       </c>
-      <c r="K11" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="44">
-        <v>0.71948008487453396</v>
-      </c>
-      <c r="N11" s="44">
-        <v>0.72509459661055797</v>
-      </c>
-      <c r="O11" s="45">
-        <v>0.01</v>
-      </c>
-      <c r="P11" s="45">
+      <c r="H148">
+        <f>N$15</f>
+        <v>0.646308558035531</v>
+      </c>
+      <c r="I148">
+        <f>N$13</f>
+        <v>0.72947401827271996</v>
+      </c>
+    </row>
+    <row r="149" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>8192</v>
+      </c>
+      <c r="C149">
+        <f>D$50</f>
+        <v>0.73435574186735098</v>
+      </c>
+      <c r="D149">
+        <f>D$48</f>
+        <v>0.73527238200424405</v>
+      </c>
+      <c r="E149" t="s">
+        <v>36</v>
+      </c>
+      <c r="F149" t="s">
+        <v>37</v>
+      </c>
+      <c r="G149">
+        <v>8192</v>
+      </c>
+      <c r="H149">
+        <f>N$50</f>
+        <v>0.68871723323832401</v>
+      </c>
+      <c r="I149">
+        <f>N$48</f>
+        <v>0.73080745544986603</v>
+      </c>
+      <c r="J149" t="s">
+        <v>36</v>
+      </c>
+      <c r="K149" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>16384</v>
+      </c>
+      <c r="C150">
+        <f>D$85</f>
+        <v>0.67389256576756495</v>
+      </c>
+      <c r="D150">
+        <f>D$83</f>
+        <v>0.73497941084274698</v>
+      </c>
+      <c r="G150">
+        <v>16384</v>
+      </c>
+      <c r="H150">
+        <f>N$85</f>
+        <v>0.63273272353864396</v>
+      </c>
+      <c r="I150">
+        <f>N$83</f>
+        <v>0.71938898103992399</v>
+      </c>
+    </row>
+    <row r="151" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>32768</v>
+      </c>
+      <c r="C151">
+        <f>D$120</f>
+        <v>0.74551247911445195</v>
+      </c>
+      <c r="D151">
+        <f>D$118</f>
+        <v>0.728751365955424</v>
+      </c>
+      <c r="G151">
+        <v>32768</v>
+      </c>
+      <c r="H151">
+        <f>N$120</f>
+        <v>0.70879909360075699</v>
+      </c>
+      <c r="I151">
+        <f>N$118</f>
+        <v>0.73686805872075301</v>
+      </c>
+    </row>
+    <row r="152" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B152">
         <v>4096</v>
       </c>
-      <c r="Q11" s="45">
-        <v>1E-3</v>
-      </c>
-      <c r="R11" s="44">
-        <v>0.71353511205545295</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="32">
-        <v>0.70766627873173005</v>
-      </c>
-      <c r="C12" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="36">
+      <c r="C152">
+        <f>I$15</f>
+        <v>0.67987259816207102</v>
+      </c>
+      <c r="D152">
+        <f>I$13</f>
+        <v>0.73164182847191905</v>
+      </c>
+      <c r="G152">
+        <v>4096</v>
+      </c>
+      <c r="H152">
+        <f>S$15</f>
+        <v>0.62863782459370598</v>
+      </c>
+      <c r="I152">
+        <f>S$13</f>
+        <v>0.71597035160206501</v>
+      </c>
+    </row>
+    <row r="153" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B153">
         <v>8192</v>
       </c>
-      <c r="E12" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="F12" s="32">
-        <v>0.68292707627676097</v>
-      </c>
-      <c r="H12" s="32">
-        <v>0.72019931651998004</v>
-      </c>
-      <c r="I12" s="36">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J12" s="36">
+      <c r="C153">
+        <f>I$50</f>
+        <v>0.66429682857991601</v>
+      </c>
+      <c r="D153">
+        <f>I$48</f>
+        <v>0.72752111674156195</v>
+      </c>
+      <c r="E153" t="s">
+        <v>39</v>
+      </c>
+      <c r="F153" t="s">
+        <v>37</v>
+      </c>
+      <c r="G153">
         <v>8192</v>
       </c>
-      <c r="K12" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="32">
-        <v>0.715037776771553</v>
-      </c>
-      <c r="N12" s="32">
-        <v>0.71643501010377797</v>
-      </c>
-      <c r="O12" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="P12" s="36">
-        <v>8192</v>
-      </c>
-      <c r="Q12" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="R12" s="32">
-        <v>0.73725322886323696</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="33">
-        <v>0.67954447535688201</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="36">
+      <c r="H153">
+        <f>S$50</f>
+        <v>0.66562935022493797</v>
+      </c>
+      <c r="I153">
+        <f>S$48</f>
+        <v>0.72296078753881898</v>
+      </c>
+      <c r="J153" t="s">
+        <v>39</v>
+      </c>
+      <c r="K153" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="154" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B154">
         <v>16384</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="33">
-        <v>0.68222465300595203</v>
-      </c>
-      <c r="H13" s="33">
-        <v>0.74200267471655701</v>
-      </c>
-      <c r="I13" s="36">
-        <v>10</v>
-      </c>
-      <c r="J13" s="36">
+      <c r="C154">
+        <f>I$85</f>
+        <v>0.68946794068504602</v>
+      </c>
+      <c r="D154">
+        <f>I$83</f>
+        <v>0.719437462952218</v>
+      </c>
+      <c r="G154">
         <v>16384</v>
       </c>
-      <c r="K13" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="L13" s="33">
-        <v>0.72069962070683302</v>
-      </c>
-      <c r="N13" s="33">
-        <v>0.75312453292742698</v>
-      </c>
-      <c r="O13" s="36">
-        <v>1</v>
-      </c>
-      <c r="P13" s="36">
-        <v>16384</v>
-      </c>
-      <c r="Q13" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="33">
-        <v>0.71549136761113297</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="34">
-        <v>0.65806453543746402</v>
-      </c>
-      <c r="C14" s="36">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D14" s="36">
+      <c r="H154">
+        <f>S$85</f>
+        <v>0.67388759889920802</v>
+      </c>
+      <c r="I154">
+        <f>S$83</f>
+        <v>0.72918125537633904</v>
+      </c>
+    </row>
+    <row r="155" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B155">
         <v>32768</v>
       </c>
-      <c r="E14" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="34">
-        <v>0.61242856827588199</v>
-      </c>
-      <c r="H14" s="34">
-        <v>0.73250635261367802</v>
-      </c>
-      <c r="I14" s="36">
-        <v>10</v>
-      </c>
-      <c r="J14" s="36">
+      <c r="C155">
+        <f>I$120</f>
+        <v>0.72035313188273697</v>
+      </c>
+      <c r="D155">
+        <f>I$118</f>
+        <v>0.74653592343395603</v>
+      </c>
+      <c r="G155">
         <v>32768</v>
       </c>
-      <c r="K14" s="36">
-        <v>1</v>
-      </c>
-      <c r="L14" s="34">
-        <v>0.72625865330656503</v>
-      </c>
-      <c r="N14" s="34">
-        <v>0.72250355026720503</v>
-      </c>
-      <c r="O14" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="P14" s="36">
-        <v>32768</v>
-      </c>
-      <c r="Q14" s="36">
-        <v>1</v>
-      </c>
-      <c r="R14" s="34">
-        <v>0.72759671930572001</v>
+      <c r="H155">
+        <f>S$120</f>
+        <v>0.69586431295312801</v>
+      </c>
+      <c r="I155">
+        <f>S$118</f>
+        <v>0.73821199293098805</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N4:N14">
+  <conditionalFormatting sqref="I148:I151">
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H148:H151">
+    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H152:H155">
     <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4:R14">
+  <conditionalFormatting sqref="I152:I155">
     <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L14">
+  <conditionalFormatting sqref="C148:C151">
     <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H14">
+  <conditionalFormatting sqref="D148:D151">
     <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F14">
+  <conditionalFormatting sqref="C152:C155">
     <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B14">
+  <conditionalFormatting sqref="D152:D155">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1826,6 +4981,604 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5444CE8-CD35-4EB5-A428-ED92A60A2BC5}">
+  <dimension ref="B2:R14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="23"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
+        <v>0.53787654224008097</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="36">
+        <v>32</v>
+      </c>
+      <c r="E4" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0.50194806170638195</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0.50620604949061798</v>
+      </c>
+      <c r="I4" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="36">
+        <v>32</v>
+      </c>
+      <c r="K4" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0.51205746388238105</v>
+      </c>
+      <c r="N4" s="24">
+        <v>0.49364470749071798</v>
+      </c>
+      <c r="O4" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P4" s="36">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="24">
+        <v>0.50497990709548901</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="25">
+        <v>0.51888184922566505</v>
+      </c>
+      <c r="C5" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="36">
+        <v>64</v>
+      </c>
+      <c r="E5" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.51944949899059201</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.53433369351518101</v>
+      </c>
+      <c r="I5" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="J5" s="36">
+        <v>64</v>
+      </c>
+      <c r="K5" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="L5" s="25">
+        <v>0.52818466098865702</v>
+      </c>
+      <c r="N5" s="25">
+        <v>0.560864808066181</v>
+      </c>
+      <c r="O5" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="P5" s="36">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="R5" s="25">
+        <v>0.53285754431889698</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="26">
+        <v>0.610294673678907</v>
+      </c>
+      <c r="C6" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="36">
+        <v>128</v>
+      </c>
+      <c r="E6" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0.53332500398919103</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0.57033623380503795</v>
+      </c>
+      <c r="I6" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="J6" s="36">
+        <v>128</v>
+      </c>
+      <c r="K6" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="L6" s="26">
+        <v>0.53488996995256799</v>
+      </c>
+      <c r="N6" s="26">
+        <v>0.583551808633887</v>
+      </c>
+      <c r="O6" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="P6" s="36">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="R6" s="26">
+        <v>0.54176305677466097</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="27">
+        <v>0.61310887218439902</v>
+      </c>
+      <c r="C7" s="36">
+        <v>10</v>
+      </c>
+      <c r="D7" s="36">
+        <v>256</v>
+      </c>
+      <c r="E7" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.59040029968531405</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.64945044609913505</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="36">
+        <v>256</v>
+      </c>
+      <c r="K7" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="L7" s="27">
+        <v>0.62286818119687304</v>
+      </c>
+      <c r="N7" s="27">
+        <v>0.63333478582543201</v>
+      </c>
+      <c r="O7" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P7" s="36">
+        <v>256</v>
+      </c>
+      <c r="Q7" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="R7" s="27">
+        <v>0.58681249297936</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41">
+        <v>0.62254876362313305</v>
+      </c>
+      <c r="C8" s="42">
+        <v>10</v>
+      </c>
+      <c r="D8" s="42">
+        <v>512</v>
+      </c>
+      <c r="E8" s="42">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="41">
+        <v>0.61549172196306701</v>
+      </c>
+      <c r="H8" s="41">
+        <v>0.65684570485080496</v>
+      </c>
+      <c r="I8" s="42">
+        <v>1E-4</v>
+      </c>
+      <c r="J8" s="42">
+        <v>512</v>
+      </c>
+      <c r="K8" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="L8" s="41">
+        <v>0.62443421273978905</v>
+      </c>
+      <c r="N8" s="41">
+        <v>0.64372310217745499</v>
+      </c>
+      <c r="O8" s="42">
+        <v>1E-4</v>
+      </c>
+      <c r="P8" s="42">
+        <v>512</v>
+      </c>
+      <c r="Q8" s="42">
+        <v>10</v>
+      </c>
+      <c r="R8" s="41">
+        <v>0.63689972433987196</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29">
+        <v>0.645481346780578</v>
+      </c>
+      <c r="C9" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="36">
+        <v>1024</v>
+      </c>
+      <c r="E9" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0.67052074001526396</v>
+      </c>
+      <c r="H9" s="29">
+        <v>0.69483838922529395</v>
+      </c>
+      <c r="I9" s="36">
+        <v>1</v>
+      </c>
+      <c r="J9" s="36">
+        <v>1024</v>
+      </c>
+      <c r="K9" s="36">
+        <v>1</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0.66266973483061897</v>
+      </c>
+      <c r="N9" s="29">
+        <v>0.709722222322271</v>
+      </c>
+      <c r="O9" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="P9" s="36">
+        <v>1024</v>
+      </c>
+      <c r="Q9" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="R9" s="29">
+        <v>0.66967553814540504</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <v>0.694987655095329</v>
+      </c>
+      <c r="C10" s="36">
+        <v>1</v>
+      </c>
+      <c r="D10" s="36">
+        <v>2048</v>
+      </c>
+      <c r="E10" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0.66531969031195404</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0.71015245992759202</v>
+      </c>
+      <c r="I10" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="J10" s="36">
+        <v>2048</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0.703051004096238</v>
+      </c>
+      <c r="N10" s="30">
+        <v>0.69871846339354704</v>
+      </c>
+      <c r="O10" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="36">
+        <v>2048</v>
+      </c>
+      <c r="Q10" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R10" s="30">
+        <v>0.72089388717042102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44">
+        <v>0.68707097943421502</v>
+      </c>
+      <c r="C11" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="45">
+        <v>4096</v>
+      </c>
+      <c r="E11" s="45">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F11" s="44">
+        <v>0.67799559054648895</v>
+      </c>
+      <c r="H11" s="44">
+        <v>0.71692056356342004</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="45">
+        <v>4096</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="44">
+        <v>0.71948008487453396</v>
+      </c>
+      <c r="N11" s="44">
+        <v>0.72509459661055797</v>
+      </c>
+      <c r="O11" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="P11" s="45">
+        <v>4096</v>
+      </c>
+      <c r="Q11" s="45">
+        <v>1E-3</v>
+      </c>
+      <c r="R11" s="44">
+        <v>0.71353511205545295</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="32">
+        <v>0.70766627873173005</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="36">
+        <v>8192</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0.68292707627676097</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0.72019931651998004</v>
+      </c>
+      <c r="I12" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J12" s="36">
+        <v>8192</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="32">
+        <v>0.715037776771553</v>
+      </c>
+      <c r="N12" s="32">
+        <v>0.71643501010377797</v>
+      </c>
+      <c r="O12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="36">
+        <v>8192</v>
+      </c>
+      <c r="Q12" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="R12" s="32">
+        <v>0.73725322886323696</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="33">
+        <v>0.67954447535688201</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="36">
+        <v>16384</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0.68222465300595203</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0.74200267471655701</v>
+      </c>
+      <c r="I13" s="36">
+        <v>10</v>
+      </c>
+      <c r="J13" s="36">
+        <v>16384</v>
+      </c>
+      <c r="K13" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="L13" s="33">
+        <v>0.72069962070683302</v>
+      </c>
+      <c r="N13" s="33">
+        <v>0.75312453292742698</v>
+      </c>
+      <c r="O13" s="36">
+        <v>1</v>
+      </c>
+      <c r="P13" s="36">
+        <v>16384</v>
+      </c>
+      <c r="Q13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" s="33">
+        <v>0.71549136761113297</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="34">
+        <v>0.65806453543746402</v>
+      </c>
+      <c r="C14" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D14" s="36">
+        <v>32768</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0.61242856827588199</v>
+      </c>
+      <c r="H14" s="34">
+        <v>0.73250635261367802</v>
+      </c>
+      <c r="I14" s="36">
+        <v>10</v>
+      </c>
+      <c r="J14" s="36">
+        <v>32768</v>
+      </c>
+      <c r="K14" s="36">
+        <v>1</v>
+      </c>
+      <c r="L14" s="34">
+        <v>0.72625865330656503</v>
+      </c>
+      <c r="N14" s="34">
+        <v>0.72250355026720503</v>
+      </c>
+      <c r="O14" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" s="36">
+        <v>32768</v>
+      </c>
+      <c r="Q14" s="36">
+        <v>1</v>
+      </c>
+      <c r="R14" s="34">
+        <v>0.72759671930572001</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N4:N14">
+    <cfRule type="top10" dxfId="13" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R14">
+    <cfRule type="top10" dxfId="12" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L14">
+    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H14">
+    <cfRule type="top10" dxfId="10" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F14">
+    <cfRule type="top10" dxfId="9" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B14">
+    <cfRule type="top10" dxfId="8" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V310"/>
   <sheetViews>
@@ -5786,7 +9539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V311"/>
   <sheetViews>
@@ -10062,7 +13815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99781522-36EF-4744-8B68-C6A7EF0D301F}">
   <dimension ref="A1:V310"/>
   <sheetViews>

</xml_diff>